<commit_message>
First pass at adding POIs to town map. Seems to corrupt my local when switching from town with POIs to one without.
</commit_message>
<xml_diff>
--- a/data/StateWQData.xlsx
+++ b/data/StateWQData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kk4si\PycharmProjects\wq-dashboard\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kk4si\PycharmProjects\wandrerQuest\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71C353FD-A8E9-4B8E-87BE-365E8FEABD14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E44534ED-D0FF-4B4F-9882-00E052C03E79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="7890" windowWidth="29040" windowHeight="15720" xr2:uid="{5FB156D7-5DC8-4408-98DA-B4BF9A423E20}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10260" xr2:uid="{5FB156D7-5DC8-4408-98DA-B4BF9A423E20}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="56">
   <si>
     <t>State</t>
   </si>
@@ -210,6 +210,18 @@
   </si>
   <si>
     <t>1drv.ms/x/s!An0k-SnslkINga9KpqflWxEJBY0F3Q?e=QrQrkX</t>
+  </si>
+  <si>
+    <t>StateHistoricalMarkerFileName</t>
+  </si>
+  <si>
+    <t>StateHistoricalMarkerOneDriveLink</t>
+  </si>
+  <si>
+    <t>NH Historical Highway Markers.2.xlsx</t>
+  </si>
+  <si>
+    <t>1drv.ms/x/s!An0k-SnslkINzx1beYrxBM-Rlm6j?e=mS31Zx</t>
   </si>
 </sst>
 </file>
@@ -581,11 +593,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7FF1582-0A37-4164-9A09-BF5441CF4454}">
-  <dimension ref="A1:P20"/>
+  <dimension ref="A1:R20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I11" sqref="I11"/>
+      <selection pane="bottomLeft" activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -601,9 +613,11 @@
     <col min="11" max="11" width="24.5" customWidth="1"/>
     <col min="12" max="14" width="55.6796875" customWidth="1"/>
     <col min="15" max="15" width="51.31640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="31" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="29.58984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -652,8 +666,14 @@
       <c r="P1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.75">
+      <c r="Q1" t="s">
+        <v>52</v>
+      </c>
+      <c r="R1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -694,7 +714,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -717,7 +737,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.75">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -740,7 +760,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.75">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -763,7 +783,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.75">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -786,7 +806,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.75">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -809,7 +829,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.75">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -832,7 +852,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.75">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -878,8 +898,14 @@
       <c r="P9" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.75">
+      <c r="Q9" t="s">
+        <v>54</v>
+      </c>
+      <c r="R9" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.75">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -902,7 +928,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.75">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -925,7 +951,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.75">
       <c r="A12" t="s">
         <v>5</v>
       </c>
@@ -948,7 +974,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.75">
       <c r="A13" t="s">
         <v>5</v>
       </c>
@@ -971,7 +997,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.75">
       <c r="A14" t="s">
         <v>5</v>
       </c>
@@ -994,7 +1020,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.75">
       <c r="A15" t="s">
         <v>5</v>
       </c>
@@ -1017,7 +1043,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.75">
       <c r="A16" t="s">
         <v>5</v>
       </c>

</xml_diff>